<commit_message>
Land Use Transition Classification
</commit_message>
<xml_diff>
--- a/Reclass_Collection5.xlsx
+++ b/Reclass_Collection5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annapede/Desktop/Dissertation/Dados Suporte/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7788815B-07C3-6A48-A4CD-281ABCCCAF01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD406630-C4FB-F84C-B81D-45CD1158542A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="24900" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="24900" windowHeight="16220" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classification" sheetId="1" r:id="rId1"/>
@@ -1490,17 +1490,17 @@
     <xf numFmtId="0" fontId="0" fillId="43" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1895,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1911,31 +1911,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="42" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="H1" s="54" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="H1" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="I1" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="54" t="s">
+      <c r="N1" s="53" t="s">
         <v>94</v>
       </c>
       <c r="O1" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54" t="s">
+      <c r="P1" s="55"/>
+      <c r="Q1" s="53" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1953,26 +1953,26 @@
         <v>4</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55" t="s">
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55" t="s">
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55" t="s">
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
     </row>
     <row r="3" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
@@ -1988,11 +1988,11 @@
         <v>129912</v>
       </c>
       <c r="E3" s="8"/>
-      <c r="H3" s="56">
+      <c r="H3" s="54">
         <f>C3</f>
         <v>1</v>
       </c>
-      <c r="I3" s="56">
+      <c r="I3" s="54">
         <f>C$19</f>
         <v>39</v>
       </c>
@@ -2000,11 +2000,11 @@
         <f>_xlfn.CONCAT(H3,I3)</f>
         <v>139</v>
       </c>
-      <c r="K3" s="56">
+      <c r="K3" s="54">
         <f>C16</f>
         <v>15</v>
       </c>
-      <c r="L3" s="56">
+      <c r="L3" s="54">
         <f>I3</f>
         <v>39</v>
       </c>
@@ -2012,11 +2012,11 @@
         <f>_xlfn.CONCAT(K3,L3)</f>
         <v>1539</v>
       </c>
-      <c r="N3" s="56">
+      <c r="N3" s="54">
         <f>C3</f>
         <v>1</v>
       </c>
-      <c r="O3" s="56">
+      <c r="O3" s="54">
         <f>C$15</f>
         <v>14</v>
       </c>
@@ -2024,17 +2024,11 @@
         <f>_xlfn.CONCAT(N3,O3)</f>
         <v>114</v>
       </c>
-      <c r="Q3" s="56">
-        <f>C17</f>
-        <v>18</v>
-      </c>
-      <c r="R3" s="56">
-        <f>C$19</f>
-        <v>39</v>
-      </c>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
       <c r="S3" t="str">
         <f>_xlfn.CONCAT(Q3,R3)</f>
-        <v>1839</v>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2051,11 +2045,11 @@
         <v>9</v>
       </c>
       <c r="E4" s="11"/>
-      <c r="H4" s="56">
-        <f t="shared" ref="H4:H8" si="0">C4</f>
+      <c r="H4" s="54">
+        <f t="shared" ref="H4:H7" si="0">C4</f>
         <v>2</v>
       </c>
-      <c r="I4" s="56">
+      <c r="I4" s="54">
         <f t="shared" ref="I4:I7" si="1">C$19</f>
         <v>39</v>
       </c>
@@ -2063,10 +2057,10 @@
         <f>_xlfn.CONCAT(H4,I4)</f>
         <v>239</v>
       </c>
-      <c r="N4" s="56">
+      <c r="N4" s="54">
         <v>1</v>
       </c>
-      <c r="O4" s="56">
+      <c r="O4" s="54">
         <f>C$31</f>
         <v>31</v>
       </c>
@@ -2074,11 +2068,11 @@
         <f t="shared" ref="P4:P19" si="2">_xlfn.CONCAT(N4,O4)</f>
         <v>131</v>
       </c>
-      <c r="Q4" s="56">
+      <c r="Q4" s="54">
         <f>C18</f>
         <v>19</v>
       </c>
-      <c r="R4" s="56">
+      <c r="R4" s="54">
         <f t="shared" ref="R4:R8" si="3">C$19</f>
         <v>39</v>
       </c>
@@ -2101,11 +2095,11 @@
         <v>6400</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="H5" s="56">
+      <c r="H5" s="54">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I5" s="56">
+      <c r="I5" s="54">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
@@ -2113,11 +2107,11 @@
         <f t="shared" ref="J5:J8" si="5">_xlfn.CONCAT(H5,I5)</f>
         <v>339</v>
       </c>
-      <c r="N5" s="56">
+      <c r="N5" s="54">
         <f>C4</f>
         <v>2</v>
       </c>
-      <c r="O5" s="56">
+      <c r="O5" s="54">
         <f>C$15</f>
         <v>14</v>
       </c>
@@ -2125,11 +2119,11 @@
         <f t="shared" si="2"/>
         <v>214</v>
       </c>
-      <c r="Q5" s="56">
+      <c r="Q5" s="54">
         <f>C20</f>
         <v>20</v>
       </c>
-      <c r="R5" s="56">
+      <c r="R5" s="54">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
@@ -2152,11 +2146,11 @@
         <v>14</v>
       </c>
       <c r="E6" s="15"/>
-      <c r="H6" s="56">
+      <c r="H6" s="54">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I6" s="56">
+      <c r="I6" s="54">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
@@ -2164,11 +2158,11 @@
         <f t="shared" si="5"/>
         <v>439</v>
       </c>
-      <c r="N6" s="56">
+      <c r="N6" s="54">
         <f>N5</f>
         <v>2</v>
       </c>
-      <c r="O6" s="56">
+      <c r="O6" s="54">
         <f>C$31</f>
         <v>31</v>
       </c>
@@ -2176,11 +2170,11 @@
         <f t="shared" si="2"/>
         <v>231</v>
       </c>
-      <c r="Q6" s="56">
+      <c r="Q6" s="54">
         <f>C21</f>
         <v>41</v>
       </c>
-      <c r="R6" s="56">
+      <c r="R6" s="54">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
@@ -2203,11 +2197,11 @@
         <v>687537</v>
       </c>
       <c r="E7" s="16"/>
-      <c r="H7" s="56">
+      <c r="H7" s="54">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I7" s="56">
+      <c r="I7" s="54">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
@@ -2215,11 +2209,11 @@
         <f t="shared" si="5"/>
         <v>539</v>
       </c>
-      <c r="N7" s="56">
+      <c r="N7" s="54">
         <f>C5</f>
         <v>3</v>
       </c>
-      <c r="O7" s="56">
+      <c r="O7" s="54">
         <f>C$15</f>
         <v>14</v>
       </c>
@@ -2227,11 +2221,11 @@
         <f t="shared" si="2"/>
         <v>314</v>
       </c>
-      <c r="Q7" s="56">
+      <c r="Q7" s="54">
         <f>C22</f>
         <v>36</v>
       </c>
-      <c r="R7" s="56">
+      <c r="R7" s="54">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
@@ -2254,17 +2248,17 @@
         <v>935132</v>
       </c>
       <c r="E8" s="17"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
       <c r="J8" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="N8" s="56">
+      <c r="N8" s="54">
         <f>N7</f>
         <v>3</v>
       </c>
-      <c r="O8" s="56">
+      <c r="O8" s="54">
         <f>C$31</f>
         <v>31</v>
       </c>
@@ -2272,11 +2266,11 @@
         <f t="shared" si="2"/>
         <v>331</v>
       </c>
-      <c r="Q8" s="56">
+      <c r="Q8" s="54">
         <f>C23</f>
         <v>21</v>
       </c>
-      <c r="R8" s="56">
+      <c r="R8" s="54">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
@@ -2299,12 +2293,12 @@
         <v>21</v>
       </c>
       <c r="E9" s="18"/>
-      <c r="H9" s="56"/>
-      <c r="N9" s="56">
+      <c r="H9" s="54"/>
+      <c r="N9" s="54">
         <f>C6</f>
         <v>4</v>
       </c>
-      <c r="O9" s="56">
+      <c r="O9" s="54">
         <f>C$15</f>
         <v>14</v>
       </c>
@@ -2327,11 +2321,11 @@
         <v>24</v>
       </c>
       <c r="E10" s="20"/>
-      <c r="N10" s="56">
+      <c r="N10" s="54">
         <f>N9</f>
         <v>4</v>
       </c>
-      <c r="O10" s="56">
+      <c r="O10" s="54">
         <f>C$31</f>
         <v>31</v>
       </c>
@@ -2354,11 +2348,11 @@
         <v>27</v>
       </c>
       <c r="E11" s="21"/>
-      <c r="N11" s="56">
+      <c r="N11" s="54">
         <f>C7</f>
         <v>5</v>
       </c>
-      <c r="O11" s="56">
+      <c r="O11" s="54">
         <f>C$15</f>
         <v>14</v>
       </c>
@@ -2381,11 +2375,11 @@
         <v>30</v>
       </c>
       <c r="E12" s="22"/>
-      <c r="N12" s="56">
+      <c r="N12" s="54">
         <f>N11</f>
         <v>5</v>
       </c>
-      <c r="O12" s="56">
+      <c r="O12" s="54">
         <f>C$31</f>
         <v>31</v>
       </c>
@@ -2832,7 +2826,7 @@
         <v>139</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7:B11" si="1">A2</f>
+        <f t="shared" ref="B7:B10" si="1">A2</f>
         <v>238</v>
       </c>
       <c r="C7">
@@ -3049,11 +3043,11 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="str">
-        <f t="shared" ref="A8:A12" si="1">B2</f>
+        <f t="shared" ref="A8:A11" si="1">B2</f>
         <v>231</v>
       </c>
       <c r="B8">
-        <f t="shared" ref="B8:B12" si="2">A3</f>
+        <f t="shared" ref="B8:B10" si="2">A3</f>
         <v>313</v>
       </c>
       <c r="C8">
@@ -3105,10 +3099,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0850F94A-3E42-8E4B-A976-B6EEFD866CF9}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3116,11 +3110,11 @@
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1">
         <f>B1-1</f>
-        <v>1838</v>
+        <v>1938</v>
       </c>
       <c r="B1" t="str">
-        <f>Classification!S3</f>
-        <v>1839</v>
+        <f>Classification!S4</f>
+        <v>1939</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -3128,12 +3122,12 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2">
-        <f t="shared" ref="A2:A6" si="0">B2-1</f>
-        <v>1938</v>
+        <f t="shared" ref="A2:A5" si="0">B2-1</f>
+        <v>2038</v>
       </c>
       <c r="B2" t="str">
-        <f>Classification!S4</f>
-        <v>1939</v>
+        <f>Classification!S5</f>
+        <v>2039</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3142,11 +3136,11 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3">
         <f t="shared" si="0"/>
-        <v>2038</v>
+        <v>4138</v>
       </c>
       <c r="B3" t="str">
-        <f>Classification!S5</f>
-        <v>2039</v>
+        <f>Classification!S6</f>
+        <v>4139</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3155,11 +3149,11 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4">
         <f t="shared" si="0"/>
-        <v>4138</v>
+        <v>3638</v>
       </c>
       <c r="B4" t="str">
-        <f>Classification!S6</f>
-        <v>4139</v>
+        <f>Classification!S7</f>
+        <v>3639</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3168,11 +3162,11 @@
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5">
         <f t="shared" si="0"/>
-        <v>3638</v>
+        <v>2138</v>
       </c>
       <c r="B5" t="str">
-        <f>Classification!S7</f>
-        <v>3639</v>
+        <f>Classification!S8</f>
+        <v>2139</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3180,62 +3174,53 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6">
-        <f t="shared" si="0"/>
-        <v>2138</v>
-      </c>
-      <c r="B6" t="str">
-        <f>Classification!S8</f>
-        <v>2139</v>
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>1938</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>0</v>
+        <v>1939</v>
       </c>
       <c r="B7">
-        <f>A1</f>
-        <v>1838</v>
+        <v>2038</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" t="str">
-        <f>B1</f>
-        <v>1839</v>
+      <c r="A8">
+        <v>2039</v>
       </c>
       <c r="B8">
-        <f t="shared" ref="B8:B13" si="1">A2</f>
-        <v>1938</v>
+        <v>2138</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" t="str">
-        <f t="shared" ref="A9:A17" si="2">B2</f>
-        <v>1939</v>
+      <c r="A9">
+        <v>2139</v>
       </c>
       <c r="B9">
-        <f t="shared" si="1"/>
-        <v>2038</v>
+        <v>3638</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" t="str">
-        <f t="shared" si="2"/>
-        <v>2039</v>
+      <c r="A10">
+        <v>3639</v>
       </c>
       <c r="B10">
-        <f t="shared" si="1"/>
         <v>4138</v>
       </c>
       <c r="C10">
@@ -3243,40 +3228,13 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" t="str">
-        <f t="shared" si="2"/>
+      <c r="A11">
         <v>4139</v>
       </c>
       <c r="B11">
-        <f t="shared" si="1"/>
-        <v>3638</v>
+        <v>5000</v>
       </c>
       <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" t="str">
-        <f t="shared" si="2"/>
-        <v>3639</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="1"/>
-        <v>2138</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" t="str">
-        <f t="shared" si="2"/>
-        <v>2139</v>
-      </c>
-      <c r="B13">
-        <v>4000</v>
-      </c>
-      <c r="C13">
         <v>0</v>
       </c>
     </row>

</xml_diff>